<commit_message>
prospects import example 👾
</commit_message>
<xml_diff>
--- a/database/seeders/uploads/local/prospects.xlsx
+++ b/database/seeders/uploads/local/prospects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\raul\wowsbar\database\seeders\uploads\local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AB6165-0537-4FAD-A659-BA99064EBB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57991394-BF99-40A5-AF75-DA503346F062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="690" windowWidth="26290" windowHeight="15710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="350" windowWidth="26290" windowHeight="15710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -123,21 +123,27 @@
     <t>schumm.com</t>
   </si>
   <si>
-    <t>"+60 012 9892525"</t>
-  </si>
-  <si>
     <t>rath.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +60 012 9892525</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +476,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,11 +537,11 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>